<commit_message>
Pantalla recomendaciones, llegaria desde link del correo
</commit_message>
<xml_diff>
--- a/target/classes/Excel para modulo importador.xlsx
+++ b/target/classes/Excel para modulo importador.xlsx
@@ -1,42 +1,89 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\54116\MisArchivos\3ero-UTN\Diseño de Sistemas\Huella_de_Carbono\2022-mi-no-mino-grupo-05\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DB3501-4412-420E-95B9-84836FDC55A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A13">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
-        <t xml:space="preserve">Suponemos q nos va a entregar 4 lineas seguidad de logistica de productos y residuos
-	-LEANDRO MARCELO LIENARD GUERRISI</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="B9">
-      <text>
-        <t xml:space="preserve">lts
-	-LEANDRO MARCELO LIENARD GUERRISI
-n***er
-	-THIAGO MARTIN CABRERA LAVEZZI</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="E1">
-      <text>
-        <t xml:space="preserve">• Formato MM/AAAA si corresponde
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>• Formato MM/AAAA si corresponde
 a Periodicidad mensual
 • Formato AAAA si corresponde a
 Periodicidad anual
 	-LEANDRO MARCELO LIENARD GUERRISI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Suponemos q nos va a entregar 4 lineas seguidad de logistica de productos y residuos
+	-LEANDRO MARCELO LIENARD GUERRISI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{29FBEA68-719F-4CA9-B8B5-5CE8A0F977FB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Suponemos q nos va a entregar 4 lineas seguidad de logistica de productos y residuos
+	-LEANDRO MARCELO LIENARD GUERRISI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>lts
+	-LEANDRO MARCELO LIENARD GUERRISI
+n***er
+	-THIAGO MARTIN CABRERA LAVEZZI</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -44,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>Actividad</t>
   </si>
@@ -91,12 +138,6 @@
     <t>Nafta</t>
   </si>
   <si>
-    <t>Carbón</t>
-  </si>
-  <si>
-    <t>Carbón de leña</t>
-  </si>
-  <si>
     <t>Leña</t>
   </si>
   <si>
@@ -128,34 +169,41 @@
   </si>
   <si>
     <t>Peso total transportados</t>
+  </si>
+  <si>
+    <t>Utilitario liviano</t>
+  </si>
+  <si>
+    <t>CARBÓN</t>
+  </si>
+  <si>
+    <t>CARBÓN DE LEÑA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/yyyy"/>
     <numFmt numFmtId="165" formatCode="mm/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
-    <font/>
     <font>
-      <sz val="36.0"/>
-      <color theme="1"/>
+      <sz val="10"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,54 +211,55 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="6">
-    <border/>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -219,61 +268,67 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -463,263 +518,306 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="35.88"/>
-    <col customWidth="1" min="2" max="2" width="19.0"/>
-    <col customWidth="1" min="5" max="5" width="17.63"/>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="6" t="s">
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6">
-        <v>1000.0</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="6">
-        <v>2002.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="6" t="s">
+      <c r="E3" s="2">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="6">
-        <v>2000.0</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="6">
-        <v>2001.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="s">
+      <c r="E4" s="2">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="6">
-        <v>6900.0</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="C5" s="2">
+        <v>6900</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="6">
-        <v>2002.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="s">
+      <c r="E5" s="2">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="6">
-        <v>20.0</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="C6" s="2">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="8">
-        <v>37347.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="s">
+      <c r="E6" s="4">
+        <v>37347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="6">
-        <v>420.0</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="2">
+        <v>420</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="6">
-        <v>1963.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="s">
+      <c r="E7" s="2">
+        <v>1963</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="2">
+        <v>49</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="5">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="5">
+        <v>43862</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="6">
-        <v>49.0</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="C18" s="2">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="9">
-        <v>43831.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="E18" s="5">
+        <v>43891</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="C19" s="2">
+        <v>15</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="9">
-        <v>43862.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="7" t="s">
+      <c r="E19" s="5">
+        <v>43975</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="B20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="2">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="9">
-        <v>43891.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="6">
-        <v>15.0</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="9">
-        <v>43975.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="6">
-        <v>10.0</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="8">
-        <v>44501.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="6">
-        <v>1977.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="6">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="6">
-        <v>4500.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="E25" s="10"/>
+      <c r="E20" s="4">
+        <v>44501</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -728,7 +826,7 @@
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E2"/>
   </mergeCells>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>